<commit_message>
SSP2018-19 Input file checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory SSP201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory SSP201819.xlsx
@@ -1,41 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XCD HR_Documents\Project Imp Documents\Regression Testing_2018_2019\Statutory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{94E8A3B3-6DAD-4507-9BEF-EF9F5479E08F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="15" firstSheet="13" windowHeight="7530" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="2" r:id="rId1"/>
-    <sheet name="ResetData" sheetId="13" r:id="rId2"/>
-    <sheet name="CreateMaleEmployee" sheetId="14" r:id="rId3"/>
-    <sheet name="UpdateTaxCodeAndAnnualSalary" sheetId="15" r:id="rId4"/>
-    <sheet name="ProcessPayrolFor20FourWeeklySSP" sheetId="1" r:id="rId5"/>
-    <sheet name="ProcessPayrolFor24FourWeeklySSP" sheetId="3" r:id="rId6"/>
-    <sheet name="ProcessPayrolFor28FourWeeklySSP" sheetId="4" r:id="rId7"/>
-    <sheet name="CreateLeaveRequest" sheetId="9" r:id="rId8"/>
-    <sheet name="UpdateLeaveRecord" sheetId="10" r:id="rId9"/>
-    <sheet name="AverageWeeklyEarningsTestReport" sheetId="19" r:id="rId10"/>
-    <sheet name="ProcessPayrolFor32FourWeeklySSP" sheetId="6" r:id="rId11"/>
-    <sheet name="ProcessPayrolFor36FourWeeklySSP" sheetId="7" r:id="rId12"/>
-    <sheet name="CreateLeaveRequest2" sheetId="11" r:id="rId13"/>
-    <sheet name="UpdateLeaveRecord2" sheetId="12" r:id="rId14"/>
-    <sheet name="AverageWeeklyEarningsTestReprt2" sheetId="22" r:id="rId15"/>
-    <sheet name="ProcessPayrolFor40FourWeeklySSP" sheetId="8" r:id="rId16"/>
+    <sheet name="first" r:id="rId1" sheetId="2"/>
+    <sheet name="ResetData" r:id="rId2" sheetId="13"/>
+    <sheet name="CreateMaleEmployee" r:id="rId3" sheetId="14"/>
+    <sheet name="UpdateTaxCodeAndAnnualSalary" r:id="rId4" sheetId="15"/>
+    <sheet name="ProcessPayrolFor20FourWeeklySSP" r:id="rId5" sheetId="1"/>
+    <sheet name="ProcessPayrolFor24FourWeeklySSP" r:id="rId6" sheetId="3"/>
+    <sheet name="ProcessPayrolFor28FourWeeklySSP" r:id="rId7" sheetId="4"/>
+    <sheet name="CreateLeaveRequest" r:id="rId8" sheetId="9"/>
+    <sheet name="UpdateLeaveRecord" r:id="rId9" sheetId="10"/>
+    <sheet name="AverageWeeklyEarningsTestReport" r:id="rId10" sheetId="19"/>
+    <sheet name="ProcessPayrolFor32FourWeeklySSP" r:id="rId11" sheetId="6"/>
+    <sheet name="ProcessPayrolFor36FourWeeklySSP" r:id="rId12" sheetId="7"/>
+    <sheet name="CreateLeaveRequest2" r:id="rId13" sheetId="11"/>
+    <sheet name="UpdateLeaveRecord2" r:id="rId14" sheetId="12"/>
+    <sheet name="AverageWeeklyEarningsTestReprt2" r:id="rId15" sheetId="22"/>
+    <sheet name="ProcessPayrolFor40FourWeeklySSP" r:id="rId16" sheetId="8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="190">
   <si>
     <t>EmpName</t>
   </si>
@@ -605,27 +604,13 @@
   </si>
   <si>
     <t>12/11/2018</t>
-  </si>
-  <si>
-    <t>employeeTaxable</t>
-  </si>
-  <si>
-    <t>employeeNiable</t>
-  </si>
-  <si>
-    <t>includeInHolidayEarnings</t>
-  </si>
-  <si>
-    <t>Attachable</t>
-  </si>
-  <si>
-    <t>AttachableForCouncilTax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -703,76 +688,76 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="2"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -789,10 +774,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -827,7 +812,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -879,7 +864,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -984,7 +969,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -993,13 +978,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1009,7 +994,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1018,7 +1003,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1027,7 +1012,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1037,12 +1022,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1073,7 +1058,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1092,7 +1077,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1104,20 +1089,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1134,7 +1119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27" r="2" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>167</v>
       </c>
@@ -1144,8 +1129,11 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="22.9" r="3" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>161</v>
       </c>
@@ -1155,8 +1143,11 @@
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="24.6" r="4" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>163</v>
       </c>
@@ -1167,7 +1158,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="31.15" r="5" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>165</v>
       </c>
@@ -1177,8 +1168,11 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25.9" r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1188,8 +1182,11 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1198,6 +1195,9 @@
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,8 +1210,11 @@
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="9" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1221,8 +1224,11 @@
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="10" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1232,9 +1238,11 @@
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="11" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1244,8 +1252,11 @@
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="12" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1255,11 +1266,11 @@
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="13" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1269,11 +1280,11 @@
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="14" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1282,6 +1293,9 @@
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,8 +1308,11 @@
       <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="16" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1305,8 +1322,11 @@
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1316,8 +1336,11 @@
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="18" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1327,8 +1350,11 @@
       <c r="C18" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="19" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1338,8 +1364,11 @@
       <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="20" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1349,8 +1378,11 @@
       <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="21" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>169</v>
       </c>
@@ -1360,8 +1392,11 @@
       <c r="C21" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="22" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1371,8 +1406,11 @@
       <c r="C22" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1382,15 +1420,18 @@
       <c r="C23" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1399,20 +1440,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -1456,7 +1497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>181</v>
       </c>
@@ -1498,15 +1539,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -1515,20 +1556,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -1572,7 +1613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>181</v>
       </c>
@@ -1614,14 +1655,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -1630,21 +1671,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -1688,7 +1729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>181</v>
       </c>
@@ -1730,14 +1771,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1746,16 +1787,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1784,7 +1825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="2" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
@@ -1810,12 +1851,12 @@
       <c r="I2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1824,15 +1865,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1861,7 +1902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -1887,13 +1928,13 @@
       <c r="I2" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1902,21 +1943,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -1960,7 +2001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>181</v>
       </c>
@@ -2002,37 +2043,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -2076,7 +2117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>181</v>
       </c>
@@ -2118,14 +2159,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2134,13 +2175,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2163,7 +2204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.6" r="2" s="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
@@ -2183,13 +2224,13 @@
       <c r="G2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2198,17 +2239,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -2399,7 +2440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>99</v>
       </c>
@@ -2586,15 +2627,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="D2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2603,15 +2644,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.6" r="2" s="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
@@ -2660,12 +2701,12 @@
       <c r="H2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2674,19 +2715,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -2730,7 +2771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>181</v>
       </c>
@@ -2772,15 +2813,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2789,19 +2830,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="44.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="44.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -2845,7 +2886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>181</v>
       </c>
@@ -2887,14 +2928,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2903,21 +2944,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -2961,7 +3002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>181</v>
       </c>
@@ -3003,14 +3044,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3019,16 +3060,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3060,7 +3101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="2" s="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
@@ -3089,32 +3130,30 @@
       <c r="J2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="11" width="24.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3137,28 +3176,16 @@
         <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>191</v>
+        <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="2" s="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
@@ -3180,24 +3207,13 @@
       <c r="G2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>29</v>
-      </c>
+      <c r="H2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Statutory SSP2 Input file checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory SSP201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory SSP201819.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{94E8A3B3-6DAD-4507-9BEF-EF9F5479E08F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="2" r:id="rId1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="190">
   <si>
     <t>EmpName</t>
   </si>
@@ -508,9 +507,6 @@
     <t>20</t>
   </si>
   <si>
-    <t>DO NOT TOUCH SSP Payment</t>
-  </si>
-  <si>
     <t>Four Week-32</t>
   </si>
   <si>
@@ -607,25 +603,13 @@
     <t>12/11/2018</t>
   </si>
   <si>
-    <t>employeeTaxable</t>
-  </si>
-  <si>
-    <t>employeeNiable</t>
-  </si>
-  <si>
-    <t>includeInHolidayEarnings</t>
-  </si>
-  <si>
-    <t>Attachable</t>
-  </si>
-  <si>
-    <t>AttachableForCouncilTax</t>
+    <t>DO NOT TOUCH SSP Payments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -769,7 +753,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1104,11 +1088,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,32 +1120,38 @@
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>168</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>162</v>
-      </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>134</v>
@@ -1169,13 +1159,16 @@
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>166</v>
-      </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1188,6 +1181,9 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1199,6 +1195,9 @@
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1210,6 +1209,9 @@
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1221,6 +1223,9 @@
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1232,7 +1237,9 @@
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10"/>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1244,6 +1251,9 @@
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1255,7 +1265,7 @@
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1269,7 +1279,7 @@
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1283,6 +1293,9 @@
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1294,6 +1307,9 @@
       <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1305,8 +1321,11 @@
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1316,8 +1335,11 @@
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1327,8 +1349,11 @@
       <c r="C18" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1338,8 +1363,11 @@
       <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1349,10 +1377,13 @@
       <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -1360,8 +1391,11 @@
       <c r="C21" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1371,8 +1405,11 @@
       <c r="C22" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1381,6 +1418,9 @@
       </c>
       <c r="C23" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1458,13 +1498,13 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>133</v>
@@ -1473,22 +1513,22 @@
         <v>154</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>186</v>
-      </c>
       <c r="I2" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>148</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L2" s="17" t="s">
         <v>4</v>
@@ -1498,7 +1538,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -1506,11 +1546,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,31 +1614,31 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>186</v>
-      </c>
       <c r="I2" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>148</v>
@@ -1614,18 +1654,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,31 +1730,31 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>186</v>
-      </c>
       <c r="I2" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>148</v>
@@ -1730,14 +1770,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1789,13 +1829,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>37</v>
@@ -1815,7 +1855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1866,13 +1906,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>37</v>
@@ -1893,7 +1933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1962,13 +2002,13 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>133</v>
@@ -1977,22 +2017,22 @@
         <v>154</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>186</v>
-      </c>
       <c r="I2" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>148</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L2" s="17" t="s">
         <v>4</v>
@@ -2002,18 +2042,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,31 +2118,31 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>186</v>
-      </c>
       <c r="I2" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>148</v>
@@ -2118,14 +2158,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2168,13 +2208,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>4</v>
@@ -2189,7 +2229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2586,15 +2626,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2665,7 +2705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2732,13 +2772,13 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>133</v>
@@ -2747,13 +2787,13 @@
         <v>153</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>149</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>150</v>
@@ -2772,7 +2812,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -2780,7 +2820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2847,13 +2887,13 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>133</v>
@@ -2862,16 +2902,16 @@
         <v>154</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>149</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>148</v>
@@ -2887,14 +2927,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2963,28 +3003,28 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>149</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>155</v>
@@ -3003,14 +3043,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3065,16 +3105,16 @@
         <v>10</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>188</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>37</v>
@@ -3094,11 +3134,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,11 +3150,9 @@
     <col min="5" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="34.28515625" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="11" width="24.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3137,42 +3175,30 @@
         <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>190</v>
+        <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>191</v>
+        <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>188</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>37</v>
@@ -3180,24 +3206,13 @@
       <c r="G2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>29</v>
-      </c>
+      <c r="H2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>